<commit_message>
Cambio transacción ZMM023, si no encuentra tickets de registro, avanzar a procesar tickets en estado REV.
</commit_message>
<xml_diff>
--- a/Robot Facturación Cemento/Data/Dia_Ejecucion.xlsx
+++ b/Robot Facturación Cemento/Data/Dia_Ejecucion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19365" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Dia_Ejecucion</t>
   </si>
@@ -35,25 +35,7 @@
     <t>dd/mm/aaaa</t>
   </si>
   <si>
-    <t>17/08/2022</t>
-  </si>
-  <si>
-    <t>30/08/2022</t>
-  </si>
-  <si>
-    <t>22/09/2022</t>
-  </si>
-  <si>
-    <t>26/10/2022</t>
-  </si>
-  <si>
-    <t>18/11/2022</t>
-  </si>
-  <si>
-    <t>14/12/2022</t>
-  </si>
-  <si>
-    <t>20/12/2022</t>
+    <t>18/01/2023</t>
   </si>
 </sst>
 </file>
@@ -378,7 +360,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,34 +385,22 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>

</xml_diff>